<commit_message>
Map INACTIVE and ACTIVE to 'Not started' status
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E47E67-64A0-2E46-BEF8-27F998EC0775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6625A697-D649-464A-90BF-9CE19159029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="224">
   <si>
     <t>table_name</t>
   </si>
@@ -691,10 +691,10 @@
     <t>join</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Only transform tasks with ACTIVE and INACTIVE statuses</t>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>Only transform tasks with ACTIVE and INACTIVE statuses, both of which get a value of 'Not started' for this field</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1354,13 +1354,9 @@
       <c r="E6" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="M6" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="M6" s="7"/>
       <c r="P6" s="7" t="s">
         <v>21</v>
       </c>
@@ -3034,7 +3030,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="15" t="s">
         <v>55</v>
       </c>
@@ -3048,7 +3044,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="15" t="s">
         <v>57</v>
       </c>
@@ -3062,7 +3058,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="15" t="s">
         <v>58</v>
       </c>
@@ -3076,7 +3072,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="15" t="s">
         <v>60</v>
       </c>
@@ -3090,7 +3086,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="15" t="s">
         <v>61</v>
       </c>
@@ -3104,7 +3100,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="15" t="s">
         <v>62</v>
       </c>
@@ -3118,7 +3114,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="15" t="s">
         <v>63</v>
       </c>
@@ -3132,7 +3128,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="15" t="s">
         <v>64</v>
       </c>
@@ -3146,7 +3142,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="15" t="s">
         <v>66</v>
       </c>
@@ -3160,7 +3156,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="15" t="s">
         <v>68</v>
       </c>
@@ -3174,7 +3170,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="15">
       <c r="A12" s="15" t="s">
         <v>69</v>
       </c>
@@ -3188,7 +3184,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="15">
       <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
@@ -3202,7 +3198,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="15">
       <c r="A14" s="15" t="s">
         <v>71</v>
       </c>
@@ -3216,7 +3212,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="15">
       <c r="A15" s="15" t="s">
         <v>72</v>
       </c>
@@ -3230,7 +3226,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="15">
       <c r="A16" s="15" t="s">
         <v>73</v>
       </c>
@@ -3244,7 +3240,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="15" t="s">
         <v>74</v>
       </c>
@@ -3258,7 +3254,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="15" t="s">
         <v>76</v>
       </c>
@@ -3272,7 +3268,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="15" t="s">
         <v>77</v>
       </c>
@@ -3286,7 +3282,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" s="15" t="s">
         <v>78</v>
       </c>
@@ -3300,7 +3296,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" s="15" t="s">
         <v>79</v>
       </c>
@@ -3314,7 +3310,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" s="15" t="s">
         <v>80</v>
       </c>
@@ -3328,7 +3324,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="15" t="s">
         <v>82</v>
       </c>
@@ -3342,7 +3338,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="15" t="s">
         <v>83</v>
       </c>
@@ -3356,7 +3352,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="15">
       <c r="A25" s="15" t="s">
         <v>85</v>
       </c>
@@ -3370,7 +3366,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="15">
       <c r="A26" s="15" t="s">
         <v>87</v>
       </c>
@@ -3384,7 +3380,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="15">
       <c r="A27" s="15" t="s">
         <v>88</v>
       </c>
@@ -3398,7 +3394,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" s="15" t="s">
         <v>89</v>
       </c>
@@ -3412,7 +3408,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="15">
       <c r="A29" s="15" t="s">
         <v>91</v>
       </c>
@@ -3426,7 +3422,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="15">
       <c r="A30" s="15" t="s">
         <v>93</v>
       </c>
@@ -3440,7 +3436,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" ht="15">
       <c r="A31" s="15" t="s">
         <v>94</v>
       </c>
@@ -3454,7 +3450,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" ht="15">
       <c r="A32" s="15" t="s">
         <v>95</v>
       </c>
@@ -3468,7 +3464,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" ht="15">
       <c r="A33" s="15" t="s">
         <v>96</v>
       </c>
@@ -3482,7 +3478,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="15">
       <c r="A34" s="15" t="s">
         <v>98</v>
       </c>
@@ -3496,7 +3492,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="15">
       <c r="A35" s="15" t="s">
         <v>99</v>
       </c>
@@ -3510,7 +3506,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="15">
       <c r="A36" s="15" t="s">
         <v>100</v>
       </c>
@@ -3524,7 +3520,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" ht="15">
       <c r="A37" s="15" t="s">
         <v>102</v>
       </c>
@@ -3538,7 +3534,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" ht="15">
       <c r="A38" s="15" t="s">
         <v>103</v>
       </c>
@@ -3552,7 +3548,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" ht="15">
       <c r="A39" s="15" t="s">
         <v>104</v>
       </c>
@@ -3566,7 +3562,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" ht="15">
       <c r="A40" s="15" t="s">
         <v>105</v>
       </c>
@@ -3580,7 +3576,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" ht="15">
       <c r="A41" s="15" t="s">
         <v>106</v>
       </c>
@@ -3594,7 +3590,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" ht="15">
       <c r="A42" s="15" t="s">
         <v>107</v>
       </c>
@@ -3608,7 +3604,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" ht="15">
       <c r="A43" s="15" t="s">
         <v>108</v>
       </c>
@@ -3622,7 +3618,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" ht="15">
       <c r="A44" s="15" t="s">
         <v>110</v>
       </c>
@@ -3636,7 +3632,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" ht="15">
       <c r="A45" s="15" t="s">
         <v>111</v>
       </c>
@@ -3650,7 +3646,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" ht="15">
       <c r="A46" s="15" t="s">
         <v>112</v>
       </c>
@@ -3664,7 +3660,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" ht="15">
       <c r="A47" s="15" t="s">
         <v>113</v>
       </c>
@@ -3678,7 +3674,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" ht="15">
       <c r="A48" s="15" t="s">
         <v>114</v>
       </c>
@@ -3692,7 +3688,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" ht="15">
       <c r="A49" s="15" t="s">
         <v>116</v>
       </c>
@@ -3706,7 +3702,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" ht="15">
       <c r="A50" s="15" t="s">
         <v>117</v>
       </c>
@@ -3720,7 +3716,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" ht="15">
       <c r="A51" s="15" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
Maintain original casrec status for filtering
We need the ACTIVE/INACTIVE status to remain for the Status field,
so that we can filter out any tasks with other statuses when
we do the transform. The default value is now set in the
transform script in the main migration repo.
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6625A697-D649-464A-90BF-9CE19159029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F00D23-073E-AF4E-AD08-C89EB2157A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="224">
   <si>
     <t>table_name</t>
   </si>
@@ -691,10 +691,10 @@
     <t>join</t>
   </si>
   <si>
-    <t>Not started</t>
-  </si>
-  <si>
-    <t>Only transform tasks with ACTIVE and INACTIVE statuses, both of which get a value of 'Not started' for this field</t>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Only transform tasks with ACTIVE and INACTIVE statuses, both of which get a value of 'Not started' for this field (set in the tasks.py transform)</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -862,6 +862,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,7 +1083,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1125,6 +1128,9 @@
       <c r="B2" t="s">
         <v>17</v>
       </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
       <c r="E2" t="s">
         <v>218</v>
       </c>
@@ -1158,9 +1164,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1354,9 +1360,13 @@
       <c r="E6" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
         <v>222</v>
       </c>
+      <c r="M6" s="7"/>
       <c r="P6" s="7" t="s">
         <v>21</v>
       </c>
@@ -1577,26 +1587,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="20" customFormat="1" ht="15">
-      <c r="A15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="19" t="s">
+    <row r="15" spans="1:26" s="24" customFormat="1" ht="15">
+      <c r="A15" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="19" t="b">
+      <c r="E15" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="P15" s="25" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move task select condition into spreadsheet (#82)
Only select ACTIVE and INACTIVE tasks, and set the status field
to "Not started" for all selected tasks.
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F00D23-073E-AF4E-AD08-C89EB2157A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980BF31B-5EF6-4D44-9E30-47E8215B3BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="225">
   <si>
     <t>table_name</t>
   </si>
@@ -685,16 +685,19 @@
     <t>sup_activity</t>
   </si>
   <si>
-    <t>Case</t>
-  </si>
-  <si>
     <t>join</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Only transform tasks with ACTIVE and INACTIVE statuses, both of which get a value of 'Not started' for this field (set in the tasks.py transform)</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>include_values = {"col": "Status", "values": ["ACTIVE", "INACTIVE"]}</t>
+  </si>
+  <si>
+    <t>Case, Status</t>
   </si>
 </sst>
 </file>
@@ -1082,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF42D79-4151-C94E-B150-CAB1CD330C33}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1091,7 +1094,7 @@
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="56.6640625" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1137,8 +1140,11 @@
       <c r="F2" t="s">
         <v>219</v>
       </c>
+      <c r="G2" t="s">
+        <v>223</v>
+      </c>
       <c r="H2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1152,7 +1158,7 @@
         <v>205</v>
       </c>
       <c r="E3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -1164,9 +1170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1360,18 +1366,14 @@
       <c r="E6" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="M6" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="M6" s="7"/>
       <c r="P6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="Q6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="20" customFormat="1" ht="15">

</xml_diff>

<commit_message>
Default assignee should not be 1 for tasks (#85)
There is no assignee with an ID of 1, so set the default assignee
for tasks to 2 instead.
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980BF31B-5EF6-4D44-9E30-47E8215B3BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D859382-E031-214B-8855-E9F6B7883C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -1085,7 +1085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF42D79-4151-C94E-B150-CAB1CD330C33}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -1170,9 +1170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1300,7 +1300,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>24</v>
@@ -3020,7 +3020,9 @@
   </sheetPr>
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>